<commit_message>
plate layout functional on all interactive charts. some refactoring
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>A</t>
   </si>
@@ -56,9 +56,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>fasd</t>
-  </si>
-  <si>
     <t>fdv</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>saer</t>
-  </si>
-  <si>
     <t>vad</t>
   </si>
   <si>
@@ -185,37 +179,37 @@
     <t>F</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>cva</t>
+  </si>
+  <si>
+    <t>vadaes</t>
+  </si>
+  <si>
+    <t>ser</t>
+  </si>
+  <si>
+    <t>dvase</t>
+  </si>
+  <si>
+    <t>vwscc</t>
+  </si>
+  <si>
+    <t>sefd</t>
+  </si>
+  <si>
+    <t>sdc</t>
+  </si>
+  <si>
+    <t>aserav</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
     <t>ca</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>cva</t>
-  </si>
-  <si>
-    <t>vadaes</t>
-  </si>
-  <si>
-    <t>ser</t>
-  </si>
-  <si>
-    <t>dvase</t>
-  </si>
-  <si>
-    <t>vwscc</t>
-  </si>
-  <si>
-    <t>sefd</t>
-  </si>
-  <si>
-    <t>sdc</t>
-  </si>
-  <si>
-    <t>aserav</t>
-  </si>
-  <si>
-    <t>G</t>
   </si>
   <si>
     <t>vawe</t>
@@ -291,6 +285,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -374,13 +369,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -473,283 +468,283 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="K5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="L5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="M5" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="J6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="G7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="K7" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="0" t="s">
+      <c r="L7" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="M7" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="H8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="0" t="s">
+      <c r="K8" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="L8" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="M8" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="L9" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="M9" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>